<commit_message>
Revisão dos artefatos da 2a. Entrega
</commit_message>
<xml_diff>
--- a/Requisitos 24-10.xlsx
+++ b/Requisitos 24-10.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="120" windowWidth="19995" windowHeight="7935"/>
@@ -11,12 +11,12 @@
     <sheet name="Plan2" sheetId="2" r:id="rId2"/>
     <sheet name="Plan3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="69">
   <si>
     <t>Projeto Software – PETCLIM</t>
   </si>
@@ -81,15 +81,9 @@
     <t>RE016</t>
   </si>
   <si>
-    <t>UC01</t>
-  </si>
-  <si>
     <t>UC02</t>
   </si>
   <si>
-    <t>UC03</t>
-  </si>
-  <si>
     <t>UC04</t>
   </si>
   <si>
@@ -117,21 +111,12 @@
     <t>UC12</t>
   </si>
   <si>
-    <t>UC13</t>
-  </si>
-  <si>
     <t>UC14</t>
   </si>
   <si>
-    <t>Agendar nova visita pós pre-cadastro.</t>
-  </si>
-  <si>
     <t>Agendar Visita</t>
   </si>
   <si>
-    <t>Agendar vacinas se o cachoro for recem nascido.</t>
-  </si>
-  <si>
     <t>Agendar Vacina</t>
   </si>
   <si>
@@ -144,15 +129,9 @@
     <t>Autenticar usuario</t>
   </si>
   <si>
-    <t>Exibir historico dos animais do usuario após ser autenticado</t>
-  </si>
-  <si>
     <t>Exibir historico de animal</t>
   </si>
   <si>
-    <t>Agendar um procedimento de higienização para o animal(banho, tosa).</t>
-  </si>
-  <si>
     <t>Agendar Procedimento</t>
   </si>
   <si>
@@ -165,63 +144,93 @@
     <t>Criar Agenda</t>
   </si>
   <si>
-    <t>Cria Campanha Prevenção</t>
-  </si>
-  <si>
     <t>UC</t>
   </si>
   <si>
-    <t>Cadastrar Usuarios</t>
-  </si>
-  <si>
-    <t>Campanha de prevenção a doenças/pragas. Ocorrerá uma verificação constante junto ao centro de zoonoses de pragas/doenças do municipio por bairro.</t>
-  </si>
-  <si>
-    <t>Cadastro os tipo de usuarios que irão utilizar o sistema e quais previlegios terão.</t>
-  </si>
-  <si>
-    <t>Cadastro animal(Data nascimento, peso, raça do animal, sexo animal.).
+    <t>Registra consulta no pronturio, medicamentos, exames que o veterinario solicitou.</t>
+  </si>
+  <si>
+    <t>Manter Prontuario, atualizar informações do animal/dono.</t>
+  </si>
+  <si>
+    <t>Cadastrar Cliente</t>
+  </si>
+  <si>
+    <t>Cadastro dono do animal(nome, telefone, endereço,cpf). Será criado um login e senha para que o dono possar agendar consultar/vacina pelo site.</t>
+  </si>
+  <si>
+    <t>Irá cadastrar os dados do Cliente e do Animal.</t>
+  </si>
+  <si>
+    <t>Cadastrar animal(Data nascimento, peso, raça do animal, sexo animal.).
 Criar prontuario do animal</t>
   </si>
   <si>
-    <t>Marten Prontuario</t>
-  </si>
-  <si>
-    <t>Registra consulta no pronturio, medicamentos, exames que o veterinario solicitou.</t>
-  </si>
-  <si>
-    <t>Registra Procedimentos de higieni aplicado no animal.</t>
-  </si>
-  <si>
-    <t>Manter Prontuario, atualizar informações do animal/dono.</t>
-  </si>
-  <si>
-    <t>Cadastrar Animal</t>
-  </si>
-  <si>
-    <t>Cadastrar Cliente</t>
-  </si>
-  <si>
-    <t>Criar Prontuario</t>
-  </si>
-  <si>
-    <t>Ira cadastra os dados do Cliente e do Animal.</t>
-  </si>
-  <si>
-    <t>Cadastro dono do animal(nome, telefone, endereço,cpf). Será criado um login e senha para que o dono possar agendar consultar/vacina pelo site.</t>
-  </si>
-  <si>
-    <t>Exibir Prontuario</t>
-  </si>
-  <si>
-    <t>Ira mostra as informações do Cliente e do animal cadastrados.</t>
+    <t>Cadastrar Cliente       Cadastrar Animal</t>
+  </si>
+  <si>
+    <t>UC02 UC03</t>
+  </si>
+  <si>
+    <t>Cadastrar Animal                Criar Prontuário</t>
+  </si>
+  <si>
+    <t>UC03 UC01</t>
+  </si>
+  <si>
+    <t>Irá mostrar as informações do Cliente e do animal cadastrados, bem como as informações registradas no prontuário do animal.</t>
+  </si>
+  <si>
+    <t>Exibir Prontuário</t>
+  </si>
+  <si>
+    <t>Exibir historico dos animais do cliente após ser autenticado</t>
+  </si>
+  <si>
+    <t>Cadastrar os tipos de usuarios que irão utilizar o sistema e quais previlegios terão.</t>
+  </si>
+  <si>
+    <t>Agendar vacinas se o animal for recem nascido.</t>
+  </si>
+  <si>
+    <t>Agendar um procedimento de higienização para o animal (banho, tosa).</t>
+  </si>
+  <si>
+    <t>Manter Prontuário</t>
+  </si>
+  <si>
+    <t>Registrar procedimentos de higiene aplicados no animal</t>
+  </si>
+  <si>
+    <t>Agendar nova visita após o cadastro</t>
+  </si>
+  <si>
+    <t>Manter Usuarios</t>
+  </si>
+  <si>
+    <t>Remover um animal do sistema em função de não pertencer mais ao dono (falecimento, venda, etc.)</t>
+  </si>
+  <si>
+    <t>Remover Animal</t>
+  </si>
+  <si>
+    <t>UC15</t>
+  </si>
+  <si>
+    <t>Permitir que o veterinário crie campanha de prevenção a doenças/pragas. Ocorrerá uma verificação constante junto ao centro de zoonoses de pragas/doenças do municipio por bairro. O Cliente poderá consultar as campanhas disponíveis no site.</t>
+  </si>
+  <si>
+    <t>Criar Campanha de Prevenção Consultar Campanhas</t>
+  </si>
+  <si>
+    <t>UC13 UC16</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -411,7 +420,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
@@ -441,6 +450,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -480,7 +492,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -585,7 +597,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -620,7 +631,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Escritório">
@@ -796,33 +806,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A5:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="8" customWidth="1"/>
-    <col min="2" max="2" width="91.140625" customWidth="1"/>
+    <col min="2" max="2" width="94.140625" customWidth="1"/>
     <col min="3" max="3" width="29.7109375" customWidth="1"/>
     <col min="4" max="4" width="6.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="15.75" thickBot="1">
       <c r="B5" s="11" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="15.75" thickBot="1">
       <c r="A6" s="2"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="4"/>
     </row>
-    <row r="7" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" ht="20.25" thickBot="1">
       <c r="A7" s="13" t="s">
         <v>1</v>
       </c>
@@ -830,7 +840,7 @@
       <c r="C7" s="14"/>
       <c r="D7" s="15"/>
     </row>
-    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="15.75" thickBot="1">
       <c r="A8" s="5" t="s">
         <v>2</v>
       </c>
@@ -841,254 +851,260 @@
         <v>4</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="29.25">
       <c r="A9" s="8" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" s="1" customFormat="1" ht="29.25" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" s="1" customFormat="1" ht="29.25">
       <c r="A10" s="8" t="s">
         <v>6</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="31.5" customHeight="1">
       <c r="A11" s="8" t="s">
         <v>7</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>23</v>
+        <v>48</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>52</v>
       </c>
       <c r="F11" s="12"/>
     </row>
-    <row r="12" spans="1:6" s="1" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" s="1" customFormat="1" ht="31.5" customHeight="1">
       <c r="A12" s="8" t="s">
         <v>8</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F12" s="12"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13" s="8" t="s">
         <v>9</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>35</v>
+        <v>61</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" s="1" customFormat="1">
       <c r="A14" s="8" t="s">
         <v>10</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" s="8" t="s">
         <v>11</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" s="1" customFormat="1">
       <c r="A16" s="8" t="s">
         <v>12</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" s="1" customFormat="1">
       <c r="A17" s="8" t="s">
         <v>13</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" s="1" customFormat="1">
       <c r="A18" s="8" t="s">
         <v>14</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19" s="8" t="s">
         <v>15</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20" s="8" t="s">
         <v>16</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="29.25" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="43.5">
       <c r="A21" s="8" t="s">
         <v>17</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="D21" s="16" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
       <c r="A22" s="8" t="s">
         <v>18</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
       <c r="A23" s="8" t="s">
         <v>19</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
       <c r="A24" s="8" t="s">
         <v>20</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
       <c r="A25" s="8"/>
-      <c r="B25" s="9"/>
-      <c r="C25" s="9"/>
-      <c r="D25" s="8"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B25" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
       <c r="A26" s="8"/>
       <c r="B26" s="9"/>
       <c r="C26" s="9"/>
       <c r="D26" s="8"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4">
       <c r="A27" s="8"/>
       <c r="B27" s="9"/>
       <c r="C27" s="9"/>
       <c r="D27" s="8"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4">
       <c r="D28" s="1"/>
     </row>
   </sheetData>
@@ -1102,24 +1118,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>